<commit_message>
Correction for marginalization as it wasn't working with non-consecutive index selection.
</commit_message>
<xml_diff>
--- a/data/samples/tpm/F6.xlsx
+++ b/data/samples/tpm/F6.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\oh\Academia\Computacion\Algorithms\Project\Back-\data\samples\tpm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20693393-C43B-47CE-8958-80208512FB70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666CFFF8-309E-4523-859B-37175ECF0DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5052" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{CB28D13E-8CC3-4AC6-8E02-04CA3895F7C3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CB28D13E-8CC3-4AC6-8E02-04CA3895F7C3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="A" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>